<commit_message>
iTA Testing complete and documented
</commit_message>
<xml_diff>
--- a/experiments/iTA/results/Results_rephrased.xlsx
+++ b/experiments/iTA/results/Results_rephrased.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhysb\OneDrive - The University of Colorado Denver\Spring_2021\ITA\Response_Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhysb\Git_Repositories\iTA\experiments\iTA\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9495412A-EAED-4BC8-A25A-56EC789963DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F3943C-0576-48B4-A5FB-425B8BA39F27}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-5955" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="376">
   <si>
     <t>Question</t>
   </si>
@@ -711,18 +711,6 @@
   </si>
   <si>
     <t>False positive is worse than false positive. False positive has a 5% chance that the patient has the disease. False negative has a 0.5% chance the patient does not have the disease, and a 1% chance it is not the disease at all. If the patient is in your training set, you can find out immediately whether the prediction is correct or not. But the point of the classifier is to make predictions for new patients. We do N't know what class these patients are in but we can make a prediction based on our classifier. Instead, we will take a classifier on some patients are known and then we will compute the proportion of the time our classification was correct. This proportion will serve as an estimate of the likelihood of the prediction being wrong.</t>
-  </si>
-  <si>
-    <t>Vishnu_Rate</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Acceptable</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>Question Rephrased</t>
@@ -1202,8 +1190,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1506,10 +1497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I76"/>
+  <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1521,30 +1512,31 @@
     <col min="5" max="5" width="81.42578125" customWidth="1"/>
     <col min="6" max="6" width="27.42578125" customWidth="1"/>
     <col min="7" max="7" width="28.140625" customWidth="1"/>
-    <col min="8" max="8" width="130.42578125" customWidth="1"/>
+    <col min="8" max="8" width="139.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>232</v>
-      </c>
-      <c r="D1" t="s">
-        <v>302</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1552,19 +1544,16 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D2" t="s">
-        <v>303</v>
-      </c>
-      <c r="H2" t="s">
+        <v>299</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1572,19 +1561,16 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D3" t="s">
-        <v>304</v>
-      </c>
-      <c r="H3" t="s">
+        <v>300</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I3" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1592,19 +1578,16 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D4" t="s">
-        <v>305</v>
-      </c>
-      <c r="H4" t="s">
+        <v>301</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I4" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1612,19 +1595,16 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D5" t="s">
-        <v>306</v>
-      </c>
-      <c r="H5" t="s">
+        <v>302</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I5" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1632,19 +1612,16 @@
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D6" t="s">
-        <v>307</v>
-      </c>
-      <c r="H6" t="s">
+        <v>303</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I6" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1652,19 +1629,16 @@
         <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D7" t="s">
-        <v>308</v>
-      </c>
-      <c r="H7" t="s">
+        <v>304</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I7" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1672,19 +1646,16 @@
         <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D8" t="s">
-        <v>309</v>
-      </c>
-      <c r="H8" t="s">
+        <v>305</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I8" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1692,19 +1663,16 @@
         <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D9" t="s">
-        <v>311</v>
-      </c>
-      <c r="H9" t="s">
+        <v>307</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I9" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1712,19 +1680,16 @@
         <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D10" t="s">
-        <v>312</v>
-      </c>
-      <c r="H10" t="s">
+        <v>308</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I10" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1735,16 +1700,13 @@
         <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>313</v>
-      </c>
-      <c r="H11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I11" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1752,19 +1714,16 @@
         <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D12" t="s">
-        <v>314</v>
-      </c>
-      <c r="H12" t="s">
+        <v>310</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I12" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1772,19 +1731,16 @@
         <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D13" t="s">
-        <v>315</v>
-      </c>
-      <c r="H13" t="s">
+        <v>311</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I13" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -1792,19 +1748,16 @@
         <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D14" t="s">
-        <v>316</v>
-      </c>
-      <c r="H14" t="s">
+        <v>312</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I14" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1812,19 +1765,16 @@
         <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D15" t="s">
-        <v>317</v>
-      </c>
-      <c r="H15" t="s">
+        <v>313</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I15" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -1832,19 +1782,16 @@
         <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D16" t="s">
-        <v>318</v>
-      </c>
-      <c r="H16" t="s">
+        <v>314</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I16" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -1852,19 +1799,16 @@
         <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D17" t="s">
-        <v>319</v>
-      </c>
-      <c r="H17" t="s">
+        <v>315</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I17" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -1872,19 +1816,16 @@
         <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D18" t="s">
-        <v>320</v>
-      </c>
-      <c r="H18" t="s">
+        <v>316</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="I18" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -1892,19 +1833,16 @@
         <v>55</v>
       </c>
       <c r="C19" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D19" t="s">
-        <v>321</v>
-      </c>
-      <c r="H19" t="s">
+        <v>317</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I19" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -1912,19 +1850,16 @@
         <v>58</v>
       </c>
       <c r="C20" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D20" t="s">
-        <v>322</v>
-      </c>
-      <c r="H20" t="s">
+        <v>318</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I20" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -1932,19 +1867,16 @@
         <v>61</v>
       </c>
       <c r="C21" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D21" t="s">
-        <v>323</v>
-      </c>
-      <c r="H21" t="s">
+        <v>319</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I21" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>63</v>
       </c>
@@ -1952,19 +1884,16 @@
         <v>64</v>
       </c>
       <c r="C22" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D22" t="s">
-        <v>324</v>
-      </c>
-      <c r="H22" t="s">
+        <v>320</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I22" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>66</v>
       </c>
@@ -1972,19 +1901,16 @@
         <v>67</v>
       </c>
       <c r="C23" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D23" t="s">
-        <v>325</v>
-      </c>
-      <c r="H23" t="s">
+        <v>321</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I23" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -1992,19 +1918,16 @@
         <v>70</v>
       </c>
       <c r="C24" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D24" t="s">
-        <v>326</v>
-      </c>
-      <c r="H24" t="s">
+        <v>322</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="I24" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -2012,19 +1935,16 @@
         <v>73</v>
       </c>
       <c r="C25" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D25" t="s">
-        <v>327</v>
-      </c>
-      <c r="H25" t="s">
+        <v>323</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I25" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>75</v>
       </c>
@@ -2032,19 +1952,16 @@
         <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D26" t="s">
-        <v>328</v>
-      </c>
-      <c r="H26" t="s">
+        <v>324</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="I26" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>78</v>
       </c>
@@ -2052,19 +1969,16 @@
         <v>79</v>
       </c>
       <c r="C27" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D27" t="s">
-        <v>329</v>
-      </c>
-      <c r="H27" t="s">
+        <v>325</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="I27" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>81</v>
       </c>
@@ -2072,19 +1986,16 @@
         <v>82</v>
       </c>
       <c r="C28" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="D28" t="s">
-        <v>330</v>
-      </c>
-      <c r="H28" t="s">
+        <v>326</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="I28" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>84</v>
       </c>
@@ -2092,19 +2003,16 @@
         <v>85</v>
       </c>
       <c r="C29" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D29" t="s">
-        <v>331</v>
-      </c>
-      <c r="H29" t="s">
+        <v>327</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="I29" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>87</v>
       </c>
@@ -2112,19 +2020,16 @@
         <v>88</v>
       </c>
       <c r="C30" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D30" t="s">
-        <v>332</v>
-      </c>
-      <c r="H30" t="s">
+        <v>328</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="I30" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>90</v>
       </c>
@@ -2132,19 +2037,16 @@
         <v>91</v>
       </c>
       <c r="C31" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D31" t="s">
-        <v>333</v>
-      </c>
-      <c r="H31" t="s">
+        <v>329</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="I31" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>93</v>
       </c>
@@ -2155,16 +2057,13 @@
         <v>93</v>
       </c>
       <c r="D32" t="s">
-        <v>334</v>
-      </c>
-      <c r="H32" t="s">
+        <v>330</v>
+      </c>
+      <c r="H32" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I32" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>96</v>
       </c>
@@ -2175,16 +2074,13 @@
         <v>96</v>
       </c>
       <c r="D33" t="s">
-        <v>335</v>
-      </c>
-      <c r="H33" t="s">
+        <v>331</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="I33" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>99</v>
       </c>
@@ -2192,19 +2088,16 @@
         <v>100</v>
       </c>
       <c r="C34" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D34" t="s">
-        <v>336</v>
-      </c>
-      <c r="H34" t="s">
+        <v>332</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="I34" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>102</v>
       </c>
@@ -2212,19 +2105,16 @@
         <v>103</v>
       </c>
       <c r="C35" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D35" t="s">
-        <v>337</v>
-      </c>
-      <c r="H35" t="s">
+        <v>333</v>
+      </c>
+      <c r="H35" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="I35" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>105</v>
       </c>
@@ -2232,19 +2122,16 @@
         <v>106</v>
       </c>
       <c r="C36" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D36" t="s">
-        <v>338</v>
-      </c>
-      <c r="H36" t="s">
+        <v>334</v>
+      </c>
+      <c r="H36" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="I36" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>108</v>
       </c>
@@ -2252,19 +2139,16 @@
         <v>109</v>
       </c>
       <c r="C37" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D37" t="s">
-        <v>339</v>
-      </c>
-      <c r="H37" t="s">
+        <v>335</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="I37" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>111</v>
       </c>
@@ -2272,19 +2156,16 @@
         <v>112</v>
       </c>
       <c r="C38" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D38" t="s">
-        <v>340</v>
-      </c>
-      <c r="H38" t="s">
+        <v>336</v>
+      </c>
+      <c r="H38" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="I38" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>114</v>
       </c>
@@ -2292,19 +2173,16 @@
         <v>115</v>
       </c>
       <c r="C39" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D39" t="s">
-        <v>341</v>
-      </c>
-      <c r="H39" t="s">
+        <v>337</v>
+      </c>
+      <c r="H39" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="I39" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>117</v>
       </c>
@@ -2312,19 +2190,16 @@
         <v>118</v>
       </c>
       <c r="C40" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="D40" t="s">
-        <v>342</v>
-      </c>
-      <c r="H40" t="s">
+        <v>338</v>
+      </c>
+      <c r="H40" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="I40" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>120</v>
       </c>
@@ -2332,19 +2207,16 @@
         <v>121</v>
       </c>
       <c r="C41" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D41" t="s">
-        <v>343</v>
-      </c>
-      <c r="H41" t="s">
+        <v>339</v>
+      </c>
+      <c r="H41" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="I41" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>123</v>
       </c>
@@ -2352,19 +2224,16 @@
         <v>124</v>
       </c>
       <c r="C42" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D42" t="s">
-        <v>344</v>
-      </c>
-      <c r="H42" t="s">
+        <v>340</v>
+      </c>
+      <c r="H42" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="I42" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>126</v>
       </c>
@@ -2372,19 +2241,16 @@
         <v>127</v>
       </c>
       <c r="C43" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D43" t="s">
-        <v>345</v>
-      </c>
-      <c r="H43" t="s">
+        <v>341</v>
+      </c>
+      <c r="H43" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="I43" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>129</v>
       </c>
@@ -2392,19 +2258,16 @@
         <v>130</v>
       </c>
       <c r="C44" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D44" t="s">
-        <v>346</v>
-      </c>
-      <c r="H44" t="s">
+        <v>342</v>
+      </c>
+      <c r="H44" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="I44" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>132</v>
       </c>
@@ -2412,19 +2275,16 @@
         <v>133</v>
       </c>
       <c r="C45" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D45" t="s">
-        <v>347</v>
-      </c>
-      <c r="H45" t="s">
+        <v>343</v>
+      </c>
+      <c r="H45" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="I45" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>135</v>
       </c>
@@ -2432,19 +2292,16 @@
         <v>136</v>
       </c>
       <c r="C46" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D46" t="s">
-        <v>348</v>
-      </c>
-      <c r="H46" t="s">
+        <v>344</v>
+      </c>
+      <c r="H46" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="I46" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>138</v>
       </c>
@@ -2452,19 +2309,16 @@
         <v>139</v>
       </c>
       <c r="C47" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D47" t="s">
-        <v>349</v>
-      </c>
-      <c r="H47" t="s">
+        <v>345</v>
+      </c>
+      <c r="H47" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="I47" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>141</v>
       </c>
@@ -2472,19 +2326,16 @@
         <v>142</v>
       </c>
       <c r="C48" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D48" t="s">
-        <v>350</v>
-      </c>
-      <c r="H48" t="s">
+        <v>346</v>
+      </c>
+      <c r="H48" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="I48" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>144</v>
       </c>
@@ -2492,19 +2343,16 @@
         <v>145</v>
       </c>
       <c r="C49" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D49" t="s">
-        <v>351</v>
-      </c>
-      <c r="H49" t="s">
+        <v>347</v>
+      </c>
+      <c r="H49" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="I49" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>147</v>
       </c>
@@ -2512,19 +2360,16 @@
         <v>148</v>
       </c>
       <c r="C50" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D50" t="s">
-        <v>352</v>
-      </c>
-      <c r="H50" t="s">
+        <v>348</v>
+      </c>
+      <c r="H50" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I50" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>150</v>
       </c>
@@ -2532,19 +2377,16 @@
         <v>151</v>
       </c>
       <c r="C51" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D51" t="s">
-        <v>353</v>
-      </c>
-      <c r="H51" t="s">
+        <v>349</v>
+      </c>
+      <c r="H51" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="I51" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>153</v>
       </c>
@@ -2552,19 +2394,16 @@
         <v>154</v>
       </c>
       <c r="C52" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D52" t="s">
-        <v>354</v>
-      </c>
-      <c r="H52" t="s">
+        <v>350</v>
+      </c>
+      <c r="H52" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="I52" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>156</v>
       </c>
@@ -2572,19 +2411,16 @@
         <v>157</v>
       </c>
       <c r="C53" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D53" t="s">
-        <v>355</v>
-      </c>
-      <c r="H53" t="s">
+        <v>351</v>
+      </c>
+      <c r="H53" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="I53" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>159</v>
       </c>
@@ -2592,19 +2428,16 @@
         <v>160</v>
       </c>
       <c r="C54" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D54" t="s">
-        <v>356</v>
-      </c>
-      <c r="H54" t="s">
+        <v>352</v>
+      </c>
+      <c r="H54" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="I54" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>162</v>
       </c>
@@ -2612,19 +2445,16 @@
         <v>163</v>
       </c>
       <c r="C55" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="D55" t="s">
-        <v>357</v>
-      </c>
-      <c r="H55" t="s">
+        <v>353</v>
+      </c>
+      <c r="H55" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="I55" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>165</v>
       </c>
@@ -2632,19 +2462,16 @@
         <v>166</v>
       </c>
       <c r="C56" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D56" t="s">
-        <v>358</v>
-      </c>
-      <c r="H56" t="s">
+        <v>354</v>
+      </c>
+      <c r="H56" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="I56" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>168</v>
       </c>
@@ -2655,16 +2482,13 @@
         <v>168</v>
       </c>
       <c r="D57" t="s">
-        <v>359</v>
-      </c>
-      <c r="H57" t="s">
+        <v>355</v>
+      </c>
+      <c r="H57" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I57" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>171</v>
       </c>
@@ -2672,19 +2496,16 @@
         <v>172</v>
       </c>
       <c r="C58" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D58" t="s">
-        <v>360</v>
-      </c>
-      <c r="H58" t="s">
+        <v>356</v>
+      </c>
+      <c r="H58" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="I58" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>174</v>
       </c>
@@ -2692,19 +2513,16 @@
         <v>175</v>
       </c>
       <c r="C59" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D59" t="s">
-        <v>361</v>
-      </c>
-      <c r="H59" t="s">
+        <v>357</v>
+      </c>
+      <c r="H59" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="I59" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>177</v>
       </c>
@@ -2712,19 +2530,16 @@
         <v>178</v>
       </c>
       <c r="C60" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D60" t="s">
-        <v>362</v>
-      </c>
-      <c r="H60" t="s">
+        <v>358</v>
+      </c>
+      <c r="H60" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="I60" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>180</v>
       </c>
@@ -2732,19 +2547,16 @@
         <v>181</v>
       </c>
       <c r="C61" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D61" t="s">
-        <v>363</v>
-      </c>
-      <c r="H61" t="s">
+        <v>359</v>
+      </c>
+      <c r="H61" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="I61" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>183</v>
       </c>
@@ -2752,19 +2564,16 @@
         <v>184</v>
       </c>
       <c r="C62" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D62" t="s">
-        <v>364</v>
-      </c>
-      <c r="H62" t="s">
+        <v>360</v>
+      </c>
+      <c r="H62" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="I62" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>186</v>
       </c>
@@ -2772,19 +2581,16 @@
         <v>187</v>
       </c>
       <c r="C63" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D63" t="s">
-        <v>365</v>
-      </c>
-      <c r="H63" t="s">
+        <v>361</v>
+      </c>
+      <c r="H63" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="I63" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>189</v>
       </c>
@@ -2792,19 +2598,16 @@
         <v>190</v>
       </c>
       <c r="C64" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D64" t="s">
-        <v>366</v>
-      </c>
-      <c r="H64" t="s">
+        <v>362</v>
+      </c>
+      <c r="H64" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="I64" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>192</v>
       </c>
@@ -2812,19 +2615,16 @@
         <v>193</v>
       </c>
       <c r="C65" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D65" t="s">
-        <v>367</v>
-      </c>
-      <c r="H65" t="s">
+        <v>363</v>
+      </c>
+      <c r="H65" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="I65" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>195</v>
       </c>
@@ -2832,19 +2632,16 @@
         <v>196</v>
       </c>
       <c r="C66" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D66" t="s">
-        <v>368</v>
-      </c>
-      <c r="H66" t="s">
+        <v>364</v>
+      </c>
+      <c r="H66" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="I66" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>198</v>
       </c>
@@ -2852,19 +2649,16 @@
         <v>199</v>
       </c>
       <c r="C67" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D67" t="s">
-        <v>369</v>
-      </c>
-      <c r="H67" t="s">
+        <v>365</v>
+      </c>
+      <c r="H67" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="I67" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>201</v>
       </c>
@@ -2872,19 +2666,16 @@
         <v>202</v>
       </c>
       <c r="C68" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D68" t="s">
-        <v>370</v>
-      </c>
-      <c r="H68" t="s">
+        <v>366</v>
+      </c>
+      <c r="H68" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="I68" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>204</v>
       </c>
@@ -2892,19 +2683,16 @@
         <v>205</v>
       </c>
       <c r="C69" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D69" t="s">
-        <v>371</v>
-      </c>
-      <c r="H69" t="s">
+        <v>367</v>
+      </c>
+      <c r="H69" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="I69" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>207</v>
       </c>
@@ -2912,19 +2700,16 @@
         <v>208</v>
       </c>
       <c r="C70" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D70" t="s">
-        <v>372</v>
-      </c>
-      <c r="H70" t="s">
+        <v>368</v>
+      </c>
+      <c r="H70" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="I70" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>210</v>
       </c>
@@ -2932,19 +2717,16 @@
         <v>211</v>
       </c>
       <c r="C71" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="D71" t="s">
-        <v>373</v>
-      </c>
-      <c r="H71" t="s">
+        <v>369</v>
+      </c>
+      <c r="H71" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="I71" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>213</v>
       </c>
@@ -2952,19 +2734,16 @@
         <v>214</v>
       </c>
       <c r="C72" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D72" t="s">
-        <v>374</v>
-      </c>
-      <c r="H72" t="s">
+        <v>370</v>
+      </c>
+      <c r="H72" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="I72" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>216</v>
       </c>
@@ -2972,19 +2751,16 @@
         <v>217</v>
       </c>
       <c r="C73" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D73" t="s">
-        <v>375</v>
-      </c>
-      <c r="H73" t="s">
+        <v>371</v>
+      </c>
+      <c r="H73" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="I73" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>219</v>
       </c>
@@ -2992,19 +2768,16 @@
         <v>220</v>
       </c>
       <c r="C74" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D74" t="s">
-        <v>376</v>
-      </c>
-      <c r="H74" t="s">
+        <v>372</v>
+      </c>
+      <c r="H74" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="I74" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>222</v>
       </c>
@@ -3012,19 +2785,16 @@
         <v>223</v>
       </c>
       <c r="C75" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D75" t="s">
-        <v>377</v>
-      </c>
-      <c r="H75" t="s">
+        <v>373</v>
+      </c>
+      <c r="H75" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="I75" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>225</v>
       </c>
@@ -3032,19 +2802,17 @@
         <v>226</v>
       </c>
       <c r="C76" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="D76" t="s">
-        <v>379</v>
-      </c>
-      <c r="H76" t="s">
+        <v>375</v>
+      </c>
+      <c r="H76" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="I76" t="s">
-        <v>230</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>